<commit_message>
Code aufgehübscht und Progress eingetragen
</commit_message>
<xml_diff>
--- a/ExcelProgress.xlsx
+++ b/ExcelProgress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laura/IdeaProjects/MiniMarioParty/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A4310A-4E30-A944-A3E0-8B5A751B561B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B637895A-79BB-BF4B-A4F0-18DDF375C927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{08BF3794-BBBC-AC4A-8BCC-FE4A663E2B12}"/>
   </bookViews>
@@ -511,11 +511,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp145.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp146.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp147.xml><?xml version="1.0" encoding="utf-8"?>
@@ -555,11 +555,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp155.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp156.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp157.xml><?xml version="1.0" encoding="utf-8"?>
@@ -587,11 +587,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp162.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp163.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp164.xml><?xml version="1.0" encoding="utf-8"?>
@@ -623,7 +623,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp170.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp171.xml><?xml version="1.0" encoding="utf-8"?>
@@ -799,7 +799,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp55.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp56.xml><?xml version="1.0" encoding="utf-8"?>
@@ -855,7 +855,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp68.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp69.xml><?xml version="1.0" encoding="utf-8"?>
@@ -915,7 +915,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp81.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp82.xml><?xml version="1.0" encoding="utf-8"?>
@@ -971,7 +971,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp94.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp95.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12476,7 +12476,7 @@
                   <a14:compatExt spid="_x0000_s1234"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32BFD9F5-1C2D-4A24-092E-8D83C60874BE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000D2040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>

</xml_diff>

<commit_message>
Neues Minispiel Grundgerüst gebaut. Keine Funktionalität!
</commit_message>
<xml_diff>
--- a/ExcelProgress.xlsx
+++ b/ExcelProgress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laura/IdeaProjects/MiniMarioParty/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B637895A-79BB-BF4B-A4F0-18DDF375C927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18AF28E8-3407-D54C-9F58-C1E5D2E25553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{08BF3794-BBBC-AC4A-8BCC-FE4A663E2B12}"/>
   </bookViews>
@@ -403,7 +403,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp120.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp121.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>